<commit_message>
fixed bug for numbering relative names
</commit_message>
<xml_diff>
--- a/task-list.xlsx
+++ b/task-list.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sknapp\Documents\PPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA968A09-0988-4B4B-9008-924D203DEA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4283FF87-E2A6-4614-8F8B-A81FAE1BA662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="2985" windowWidth="19860" windowHeight="10815" xr2:uid="{25CCED87-AC54-4A6F-A9B5-5AF021D23D3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25CCED87-AC54-4A6F-A9B5-5AF021D23D3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="DataValidation" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tasks!$A$1:$E$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tasks!$A$1:$E$93</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="169">
   <si>
     <t>Proband ID: allow user to assign (not case on develop-build branch)?</t>
   </si>
@@ -516,6 +516,36 @@
   </si>
   <si>
     <t>Permantly delete account recovery emails as they are sent</t>
+  </si>
+  <si>
+    <t>Bug Fix: CBC average person</t>
+  </si>
+  <si>
+    <t>Don't show CBC risk facet plot if proband never had BC or already had CBC. If proband had BC but not CBC, ensure the average person and proband penetrances are corrct.</t>
+  </si>
+  <si>
+    <t>PanelPRO model selection</t>
+  </si>
+  <si>
+    <t>Don’t list CBC as a separate 18th cancer when proband is selecting pre-specified models and make it clear that if BC is included, CBC is automatically included.</t>
+  </si>
+  <si>
+    <t>Load Testing/Server Setting Optimization</t>
+  </si>
+  <si>
+    <t>Configure server settings based on load test results</t>
+  </si>
+  <si>
+    <t>Include genes and tumor markers on pedigreejs</t>
+  </si>
+  <si>
+    <t>PedigreeJS has the capability to add genes and tumor markers under each node, just need to figure out how, see canrisk.org for example</t>
+  </si>
+  <si>
+    <t>Reports of app crashing frequently</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This like likely due to communication between the database and app server. Reducing the number of queries to the database and pushes to the database may alleviate the issue. For example, don’t get the user base more than once per session. Don't save the pedigree to the database with every tab change, etc. </t>
   </si>
 </sst>
 </file>
@@ -949,10 +979,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D1DF580-F174-4672-97FA-FE01A95A71D2}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E152"/>
+  <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,97 +1939,95 @@
       </c>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D64" s="3"/>
+        <v>164</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="D65" s="3"/>
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="D66" s="3"/>
       <c r="E66" s="3"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>49</v>
+        <v>160</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
     </row>
     <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
     </row>
     <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>44</v>
+        <v>155</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>45</v>
+        <v>156</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>35</v>
@@ -2008,58 +2036,54 @@
     </row>
     <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>51</v>
+        <v>158</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E71" s="3"/>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D72" s="3"/>
       <c r="E72" s="3"/>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>35</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="D73" s="3"/>
       <c r="E73" s="3"/>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>58</v>
+        <v>150</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>35</v>
@@ -2071,10 +2095,10 @@
         <v>30</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>35</v>
@@ -2086,10 +2110,10 @@
         <v>30</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>35</v>
@@ -2101,94 +2125,104 @@
         <v>30</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>114</v>
+        <v>3</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E77" s="3"/>
     </row>
-    <row r="78" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>121</v>
+        <v>56</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E78" s="3"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>153</v>
+        <v>42</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D79" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E79" s="3"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="6" t="s">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B80" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D81" s="3"/>
+        <v>108</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E81" s="3"/>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D82" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E82" s="3"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>70</v>
+        <v>121</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D83" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E83" s="3"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2196,36 +2230,36 @@
         <v>30</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
     </row>
-    <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B85" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-    </row>
-    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B85" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>141</v>
+        <v>73</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -2235,59 +2269,89 @@
         <v>30</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>128</v>
+        <v>62</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
     </row>
-    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>140</v>
+        <v>77</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
+      <c r="A89" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="3"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
+    <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
+    <row r="91" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
+      <c r="A92" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
+    <row r="93" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
     </row>
@@ -2704,15 +2768,50 @@
       <c r="D152" s="3"/>
       <c r="E152" s="3"/>
     </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="3"/>
+      <c r="B153" s="3"/>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3"/>
+      <c r="E153" s="3"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="3"/>
+      <c r="B154" s="3"/>
+      <c r="C154" s="3"/>
+      <c r="D154" s="3"/>
+      <c r="E154" s="3"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="3"/>
+      <c r="B155" s="3"/>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3"/>
+      <c r="E155" s="3"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="3"/>
+      <c r="B156" s="3"/>
+      <c r="C156" s="3"/>
+      <c r="D156" s="3"/>
+      <c r="E156" s="3"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="3"/>
+      <c r="B157" s="3"/>
+      <c r="C157" s="3"/>
+      <c r="D157" s="3"/>
+      <c r="E157" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E88" xr:uid="{5D1DF580-F174-4672-97FA-FE01A95A71D2}">
+  <autoFilter ref="A1:E93" xr:uid="{5D1DF580-F174-4672-97FA-FE01A95A71D2}">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:E153">
-    <sortCondition ref="A2:A153" customList="Very high,High,Mid,Low"/>
-    <sortCondition ref="D2:D153" customList="&quot;&quot;,Complete"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A64:E157">
+    <sortCondition ref="A2:A157" customList="Very high,High,Mid,Low"/>
+    <sortCondition ref="D2:D157" customList="&quot;&quot;,Complete"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D1:D1048576">

</xml_diff>

<commit_message>
updated README and task list
</commit_message>
<xml_diff>
--- a/task-list.xlsx
+++ b/task-list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sknapp\Documents\PPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sknapp\Dropbox (Partners HealthCare)\Package\PanelPRO_ShinyApp\PPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4283FF87-E2A6-4614-8F8B-A81FAE1BA662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFC4925-A793-4700-8EE8-8738428A0BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25CCED87-AC54-4A6F-A9B5-5AF021D23D3E}"/>
+    <workbookView xWindow="28680" yWindow="-240" windowWidth="29040" windowHeight="15840" xr2:uid="{25CCED87-AC54-4A6F-A9B5-5AF021D23D3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="170">
   <si>
     <t>Proband ID: allow user to assign (not case on develop-build branch)?</t>
   </si>
@@ -546,6 +546,9 @@
   </si>
   <si>
     <t xml:space="preserve">This like likely due to communication between the database and app server. Reducing the number of queries to the database and pushes to the database may alleviate the issue. For example, don’t get the user base more than once per session. Don't save the pedigree to the database with every tab change, etc. </t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -982,7 +985,7 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1957,7 @@
       </c>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>29</v>
       </c>
@@ -1964,7 +1967,9 @@
       <c r="C65" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D65" s="3"/>
+      <c r="D65" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2016,7 +2021,9 @@
       <c r="C69" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D69" s="3"/>
+      <c r="D69" s="3" t="s">
+        <v>169</v>
+      </c>
       <c r="E69" s="3"/>
     </row>
     <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>